<commit_message>
Update data (2020-05-08 v2)
Add Santé Montréal data
</commit_message>
<xml_diff>
--- a/app/data/covid19_MTL.xlsx
+++ b/app/data/covid19_MTL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\code\github\covid19mtl\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6358AB96-6C1F-4DF6-9B4A-522D573600DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DFE295-1854-492E-9791-DBEA89258BBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7220" yWindow="5850" windowWidth="31170" windowHeight="11480" tabRatio="585" activeTab="2" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
+    <workbookView xWindow="7980" yWindow="7460" windowWidth="31170" windowHeight="11480" tabRatio="585" activeTab="1" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="335">
   <si>
     <t>borough</t>
   </si>
@@ -985,79 +985,100 @@
     <t>13,9</t>
   </si>
   <si>
-    <t>12,7</t>
-  </si>
-  <si>
-    <t> 867,4</t>
-  </si>
-  <si>
     <t>1 666</t>
   </si>
   <si>
     <t>6 MAI, 18h04</t>
   </si>
   <si>
-    <t>0,9</t>
-  </si>
-  <si>
-    <t> 150,6</t>
-  </si>
-  <si>
-    <t> 129,7</t>
-  </si>
-  <si>
-    <t> 257,4</t>
-  </si>
-  <si>
-    <t> 587,7</t>
-  </si>
-  <si>
     <t>12,2</t>
-  </si>
-  <si>
-    <t> 660,2</t>
-  </si>
-  <si>
-    <t> 892,8</t>
   </si>
   <si>
     <t>* 4,3</t>
   </si>
   <si>
-    <t> 885,2</t>
-  </si>
-  <si>
-    <t>* 11,3</t>
-  </si>
-  <si>
     <t>8,8</t>
-  </si>
-  <si>
-    <t> 725,9</t>
-  </si>
-  <si>
-    <t> 54,9</t>
-  </si>
-  <si>
-    <t> 1 182,4</t>
-  </si>
-  <si>
-    <t> 189,4</t>
   </si>
   <si>
     <t>27,6</t>
   </si>
   <si>
-    <t> 4 878,2</t>
+    <t> 892,4</t>
   </si>
   <si>
-    <t>1 228</t>
+    <t>7 MAI, 18h04</t>
   </si>
   <si>
-    <t> 1 215,3</t>
+    <t>100 000</t>
   </si>
   <si>
-    <t> 80,7</t>
+    <t>NOMBRE DE CAS CONFIRMÉS¹</t>
+  </si>
+  <si>
+    <t>RÉPARTITION DES CAS (%)</t>
+  </si>
+  <si>
+    <t>TAUX POUR</t>
+  </si>
+  <si>
+    <t>PERSONNES</t>
+  </si>
+  <si>
+    <t>NOMBRE DE DÉCÈS</t>
+  </si>
+  <si>
+    <t>TAUX DE MORTALITÉ POUR</t>
+  </si>
+  <si>
+    <t>1,0</t>
+  </si>
+  <si>
+    <t> 157,8</t>
+  </si>
+  <si>
+    <t> 133,4</t>
+  </si>
+  <si>
+    <t> 265,5</t>
+  </si>
+  <si>
+    <t> 603,2</t>
+  </si>
+  <si>
+    <t> 680,3</t>
+  </si>
+  <si>
+    <t>914,3</t>
+  </si>
+  <si>
+    <t>12,8</t>
+  </si>
+  <si>
+    <t>912,5</t>
+  </si>
+  <si>
+    <t>* 12,1</t>
+  </si>
+  <si>
+    <t> 749</t>
+  </si>
+  <si>
+    <t> 56,8</t>
+  </si>
+  <si>
+    <t> 1 219,1</t>
+  </si>
+  <si>
+    <t> 196,3</t>
+  </si>
+  <si>
+    <t>5 015,8</t>
+  </si>
+  <si>
+    <t> 1 259,9</t>
+  </si>
+  <si>
+    <t> 83,6</t>
   </si>
 </sst>
 </file>
@@ -1571,20 +1592,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5D96B4-0147-4A32-9FAF-C932A9839F40}">
-  <dimension ref="A1:AN35"/>
+  <dimension ref="A1:AO35"/>
   <sheetViews>
     <sheetView topLeftCell="R10" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="AN36" sqref="AN36"/>
+      <selection activeCell="AN1" sqref="AN1:AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="42.453125" customWidth="1"/>
     <col min="2" max="17" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="40" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="41" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1705,8 +1726,11 @@
       <c r="AN1" s="19">
         <v>43957</v>
       </c>
+      <c r="AO1" s="19">
+        <v>43958</v>
+      </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1827,8 +1851,11 @@
       <c r="AN2">
         <v>1442</v>
       </c>
+      <c r="AO2">
+        <v>1502</v>
+      </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1949,8 +1976,11 @@
       <c r="AN3">
         <v>398</v>
       </c>
+      <c r="AO3">
+        <v>409</v>
+      </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -2071,8 +2101,11 @@
       <c r="AN4">
         <v>10</v>
       </c>
+      <c r="AO4">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -2193,8 +2226,11 @@
       <c r="AN5">
         <v>46</v>
       </c>
+      <c r="AO5">
+        <v>45</v>
+      </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2315,8 +2351,11 @@
       <c r="AN6">
         <v>1478</v>
       </c>
+      <c r="AO6">
+        <v>1512</v>
+      </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -2437,8 +2476,11 @@
       <c r="AN7">
         <v>390</v>
       </c>
+      <c r="AO7">
+        <v>393</v>
+      </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -2559,8 +2601,11 @@
       <c r="AN8">
         <v>271</v>
       </c>
+      <c r="AO8">
+        <v>274</v>
+      </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -2681,8 +2726,11 @@
       <c r="AN9">
         <v>137</v>
       </c>
+      <c r="AO9">
+        <v>141</v>
+      </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -2803,8 +2851,11 @@
       <c r="AN10">
         <v>42</v>
       </c>
+      <c r="AO10">
+        <v>42</v>
+      </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -2925,8 +2976,11 @@
       <c r="AN11">
         <v>77</v>
       </c>
+      <c r="AO11">
+        <v>77</v>
+      </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3047,8 +3101,11 @@
       <c r="AN12">
         <v>378</v>
       </c>
+      <c r="AO12">
+        <v>386</v>
+      </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3169,8 +3226,11 @@
       <c r="AN13">
         <v>888</v>
       </c>
+      <c r="AO13">
+        <v>902</v>
+      </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -3291,8 +3351,11 @@
       <c r="AN14">
         <v>118</v>
       </c>
+      <c r="AO14">
+        <v>125</v>
+      </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3413,8 +3476,11 @@
       <c r="AN15">
         <v>1341</v>
       </c>
+      <c r="AO15">
+        <v>1402</v>
+      </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -3535,8 +3601,11 @@
       <c r="AN16">
         <v>24</v>
       </c>
+      <c r="AO16">
+        <v>24</v>
+      </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3657,8 +3726,11 @@
       <c r="AN17">
         <v>1615</v>
       </c>
+      <c r="AO17">
+        <v>1676</v>
+      </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -3779,8 +3851,11 @@
       <c r="AN18">
         <v>14</v>
       </c>
+      <c r="AO18">
+        <v>15</v>
+      </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -3901,8 +3976,11 @@
       <c r="AN19">
         <v>202</v>
       </c>
+      <c r="AO19">
+        <v>207</v>
+      </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -4023,8 +4101,11 @@
       <c r="AN20">
         <v>215</v>
       </c>
+      <c r="AO20">
+        <v>217</v>
+      </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -4145,8 +4226,11 @@
       <c r="AN21">
         <v>324</v>
       </c>
+      <c r="AO21">
+        <v>337</v>
+      </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -4267,8 +4351,11 @@
       <c r="AN22">
         <v>649</v>
       </c>
+      <c r="AO22">
+        <v>657</v>
+      </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -4389,8 +4476,11 @@
       <c r="AN23">
         <v>142</v>
       </c>
+      <c r="AO23">
+        <v>142</v>
+      </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -4511,8 +4601,11 @@
       <c r="AN24">
         <v>1300</v>
       </c>
+      <c r="AO24">
+        <v>1361</v>
+      </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -4633,8 +4726,11 @@
       <c r="AN25">
         <v>978</v>
       </c>
+      <c r="AO25">
+        <v>1016</v>
+      </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>108</v>
       </c>
@@ -4755,8 +4851,11 @@
       <c r="AN26">
         <v>16</v>
       </c>
+      <c r="AO26">
+        <v>15</v>
+      </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -4877,8 +4976,11 @@
       <c r="AN27">
         <v>645</v>
       </c>
+      <c r="AO27">
+        <v>654</v>
+      </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -4999,8 +5101,11 @@
       <c r="AN28">
         <v>694</v>
       </c>
+      <c r="AO28">
+        <v>716</v>
+      </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>107</v>
       </c>
@@ -5121,8 +5226,11 @@
       <c r="AN29">
         <v>2</v>
       </c>
+      <c r="AO29">
+        <v>2</v>
+      </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -5243,8 +5351,11 @@
       <c r="AN30">
         <v>694</v>
       </c>
+      <c r="AO30">
+        <v>708</v>
+      </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -5365,8 +5476,11 @@
       <c r="AN31">
         <v>738</v>
       </c>
+      <c r="AO31">
+        <v>746</v>
+      </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -5487,8 +5601,11 @@
       <c r="AN32">
         <v>475</v>
       </c>
+      <c r="AO32">
+        <v>495</v>
+      </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -5609,8 +5726,11 @@
       <c r="AN33">
         <v>1268</v>
       </c>
+      <c r="AO33">
+        <v>1307</v>
+      </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -5731,8 +5851,11 @@
       <c r="AN34">
         <v>143</v>
       </c>
+      <c r="AO34">
+        <v>143</v>
+      </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -5852,6 +5975,9 @@
       </c>
       <c r="AN35">
         <v>765</v>
+      </c>
+      <c r="AO35">
+        <v>777</v>
       </c>
     </row>
   </sheetData>
@@ -5862,11 +5988,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2135A11-D06E-4452-A066-9CB8F334EEDF}">
-  <dimension ref="A1:AN34"/>
+  <dimension ref="A1:AO34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP11" sqref="AP11"/>
+      <selection pane="topRight" activeCell="AP1" sqref="AP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5874,10 +6000,10 @@
     <col min="1" max="1" width="40.08984375" customWidth="1"/>
     <col min="2" max="16" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="17" max="27" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="28" max="40" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="41" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6019,8 +6145,11 @@
       <c r="AN1" s="1">
         <v>43957</v>
       </c>
+      <c r="AO1" s="1">
+        <v>43958</v>
+      </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6176,8 +6305,12 @@
         <f>cases!AN2/(population_2016!$B2/1000)</f>
         <v>10.741554620283809</v>
       </c>
+      <c r="AO2" s="3">
+        <f>cases!AO2/(population_2016!$B2/1000)</f>
+        <v>11.188498640545271</v>
+      </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6333,8 +6466,12 @@
         <f>cases!AN3/(population_2016!$B3/1000)</f>
         <v>9.2999345733246095</v>
       </c>
+      <c r="AO3" s="3">
+        <f>cases!AO3/(population_2016!$B3/1000)</f>
+        <v>9.5569679409290593</v>
+      </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -6490,8 +6627,12 @@
         <f>cases!AN4/(population_2016!$B4/1000)</f>
         <v>2.6157467957101752</v>
       </c>
+      <c r="AO4" s="3">
+        <f>cases!AO4/(population_2016!$B4/1000)</f>
+        <v>2.8773214752811929</v>
+      </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -6647,8 +6788,12 @@
         <f>cases!AN5/(population_2016!$B5/1000)</f>
         <v>2.3804595321879525</v>
       </c>
+      <c r="AO5" s="3">
+        <f>cases!AO5/(population_2016!$B5/1000)</f>
+        <v>2.3287104119229971</v>
+      </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -6804,8 +6949,12 @@
         <f>cases!AN6/(population_2016!$B6/1000)</f>
         <v>8.8758107134278159</v>
       </c>
+      <c r="AO6" s="3">
+        <f>cases!AO6/(population_2016!$B6/1000)</f>
+        <v>9.079990391544559</v>
+      </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -6961,8 +7110,12 @@
         <f>cases!AN7/(population_2016!$B7/1000)</f>
         <v>12.019230769230768</v>
       </c>
+      <c r="AO7" s="3">
+        <f>cases!AO7/(population_2016!$B7/1000)</f>
+        <v>12.111686390532544</v>
+      </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -7118,8 +7271,12 @@
         <f>cases!AN8/(population_2016!$B8/1000)</f>
         <v>5.5420356244503974</v>
       </c>
+      <c r="AO8" s="3">
+        <f>cases!AO8/(population_2016!$B8/1000)</f>
+        <v>5.6033865723225427</v>
+      </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -7275,8 +7432,12 @@
         <f>cases!AN9/(population_2016!$B9/1000)</f>
         <v>7.2181243414120129</v>
       </c>
+      <c r="AO9" s="3">
+        <f>cases!AO9/(population_2016!$B9/1000)</f>
+        <v>7.4288724973656475</v>
+      </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -7432,8 +7593,12 @@
         <f>cases!AN10/(population_2016!$B10/1000)</f>
         <v>6.0232324680912095</v>
       </c>
+      <c r="AO10" s="3">
+        <f>cases!AO10/(population_2016!$B10/1000)</f>
+        <v>6.0232324680912095</v>
+      </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -7589,8 +7754,12 @@
         <f>cases!AN11/(population_2016!$B11/1000)</f>
         <v>3.8211503151208377</v>
       </c>
+      <c r="AO11" s="3">
+        <f>cases!AO11/(population_2016!$B11/1000)</f>
+        <v>3.8211503151208377</v>
+      </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -7746,8 +7915,12 @@
         <f>cases!AN12/(population_2016!$B12/1000)</f>
         <v>8.4964822765177921</v>
       </c>
+      <c r="AO12" s="3">
+        <f>cases!AO12/(population_2016!$B12/1000)</f>
+        <v>8.6763020072377444</v>
+      </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -7903,8 +8076,12 @@
         <f>cases!AN13/(population_2016!$B13/1000)</f>
         <v>11.554526173343918</v>
       </c>
+      <c r="AO13" s="3">
+        <f>cases!AO13/(population_2016!$B13/1000)</f>
+        <v>11.736692126527267</v>
+      </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -8060,8 +8237,12 @@
         <f>cases!AN14/(population_2016!$B14/1000)</f>
         <v>6.4085157225873024</v>
       </c>
+      <c r="AO14" s="3">
+        <f>cases!AO14/(population_2016!$B14/1000)</f>
+        <v>6.7886819095204478</v>
+      </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -8217,8 +8398,12 @@
         <f>cases!AN15/(population_2016!$B15/1000)</f>
         <v>9.858554372757748</v>
       </c>
+      <c r="AO15" s="3">
+        <f>cases!AO15/(population_2016!$B15/1000)</f>
+        <v>10.3070046462389</v>
+      </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>112</v>
       </c>
@@ -8374,8 +8559,12 @@
         <f>cases!AN16/(population_2016!$B16/1000)</f>
         <v>6.2337662337662341</v>
       </c>
+      <c r="AO16" s="3">
+        <f>cases!AO16/(population_2016!$B16/1000)</f>
+        <v>6.2337662337662341</v>
+      </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -8531,8 +8720,12 @@
         <f>cases!AN17/(population_2016!$B17/1000)</f>
         <v>19.17278058741126</v>
       </c>
+      <c r="AO17" s="3">
+        <f>cases!AO17/(population_2016!$B17/1000)</f>
+        <v>19.896953724149395</v>
+      </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -8688,8 +8881,12 @@
         <f>cases!AN18/(population_2016!$B18/1000)</f>
         <v>2.7722772277227725</v>
       </c>
+      <c r="AO18" s="3">
+        <f>cases!AO18/(population_2016!$B18/1000)</f>
+        <v>2.9702970297029703</v>
+      </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -8845,8 +9042,12 @@
         <f>cases!AN19/(population_2016!$B19/1000)</f>
         <v>9.962517261787335</v>
       </c>
+      <c r="AO19" s="3">
+        <f>cases!AO19/(population_2016!$B19/1000)</f>
+        <v>10.209114223712763</v>
+      </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -9002,8 +9203,12 @@
         <f>cases!AN20/(population_2016!$B20/1000)</f>
         <v>8.9755364448526347</v>
       </c>
+      <c r="AO20" s="3">
+        <f>cases!AO20/(population_2016!$B20/1000)</f>
+        <v>9.059029807130333</v>
+      </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -9159,8 +9364,12 @@
         <f>cases!AN21/(population_2016!$B21/1000)</f>
         <v>4.6755270790943335</v>
       </c>
+      <c r="AO21" s="3">
+        <f>cases!AO21/(population_2016!$B21/1000)</f>
+        <v>4.8631253878234268</v>
+      </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -9316,8 +9525,12 @@
         <f>cases!AN22/(population_2016!$B22/1000)</f>
         <v>6.240384615384615</v>
       </c>
+      <c r="AO22" s="3">
+        <f>cases!AO22/(population_2016!$B22/1000)</f>
+        <v>6.3173076923076925</v>
+      </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -9473,8 +9686,12 @@
         <f>cases!AN23/(population_2016!$B23/1000)</f>
         <v>4.5251752708731674</v>
       </c>
+      <c r="AO23" s="3">
+        <f>cases!AO23/(population_2016!$B23/1000)</f>
+        <v>4.5251752708731674</v>
+      </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -9630,8 +9847,12 @@
         <f>cases!AN24/(population_2016!$B24/1000)</f>
         <v>12.178784557301181</v>
       </c>
+      <c r="AO24" s="3">
+        <f>cases!AO24/(population_2016!$B24/1000)</f>
+        <v>12.750250601913006</v>
+      </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -9787,8 +10008,12 @@
         <f>cases!AN25/(population_2016!$B25/1000)</f>
         <v>7.0062325381474313</v>
       </c>
+      <c r="AO25" s="3">
+        <f>cases!AO25/(population_2016!$B25/1000)</f>
+        <v>7.278458342288129</v>
+      </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>108</v>
       </c>
@@ -9944,8 +10169,12 @@
         <f>cases!AN26/(population_2016!$B26/1000)</f>
         <v>3.227107704719645</v>
       </c>
+      <c r="AO26" s="3">
+        <f>cases!AO26/(population_2016!$B26/1000)</f>
+        <v>3.0254134731746669</v>
+      </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -10101,8 +10330,12 @@
         <f>cases!AN27/(population_2016!$B27/1000)</f>
         <v>6.5264904682883396</v>
       </c>
+      <c r="AO27" s="3">
+        <f>cases!AO27/(population_2016!$B27/1000)</f>
+        <v>6.6175577771481766</v>
+      </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -10258,8 +10491,12 @@
         <f>cases!AN28/(population_2016!$B28/1000)</f>
         <v>8.8627801545239766</v>
       </c>
+      <c r="AO28" s="3">
+        <f>cases!AO28/(population_2016!$B28/1000)</f>
+        <v>9.1437328395377051</v>
+      </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>107</v>
       </c>
@@ -10415,8 +10652,12 @@
         <f>cases!AN29/(population_2016!$B29/1000)</f>
         <v>2.1715526601520088</v>
       </c>
+      <c r="AO29" s="3">
+        <f>cases!AO29/(population_2016!$B29/1000)</f>
+        <v>2.1715526601520088</v>
+      </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -10572,8 +10813,12 @@
         <f>cases!AN30/(population_2016!$B30/1000)</f>
         <v>8.8802446545789557</v>
       </c>
+      <c r="AO30" s="3">
+        <f>cases!AO30/(population_2016!$B30/1000)</f>
+        <v>9.0593850366597994</v>
+      </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -10729,8 +10974,12 @@
         <f>cases!AN31/(population_2016!$B31/1000)</f>
         <v>10.660272429184301</v>
       </c>
+      <c r="AO31" s="3">
+        <f>cases!AO31/(population_2016!$B31/1000)</f>
+        <v>10.775830937901747</v>
+      </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -10886,8 +11135,12 @@
         <f>cases!AN32/(population_2016!$B32/1000)</f>
         <v>5.3269036671526298</v>
       </c>
+      <c r="AO32" s="3">
+        <f>cases!AO32/(population_2016!$B32/1000)</f>
+        <v>5.551194347874846</v>
+      </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -11043,8 +11296,12 @@
         <f>cases!AN33/(population_2016!$B33/1000)</f>
         <v>8.814553745837765</v>
       </c>
+      <c r="AO33" s="3">
+        <f>cases!AO33/(population_2016!$B33/1000)</f>
+        <v>9.0856638373895571</v>
+      </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -11198,6 +11455,10 @@
       </c>
       <c r="AN34" s="3">
         <f>cases!AN34/(population_2016!$B34/1000)</f>
+        <v>7.040173296573454</v>
+      </c>
+      <c r="AO34" s="3">
+        <f>cases!AO34/(population_2016!$B34/1000)</f>
         <v>7.040173296573454</v>
       </c>
     </row>
@@ -11210,9 +11471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9609F4-1A5A-459D-8297-63DB4B7007A3}">
   <dimension ref="A1:AS55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
+      <selection pane="bottomLeft" activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13762,11 +14023,11 @@
       </c>
       <c r="B19" s="17">
         <f>mtl_newcases!C20</f>
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="C19" s="17">
         <f t="shared" si="0"/>
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>101</v>
@@ -13932,11 +14193,11 @@
       </c>
       <c r="B20" s="17">
         <f>mtl_newcases!C21</f>
-        <v>2956</v>
+        <v>2954</v>
       </c>
       <c r="C20" s="17">
         <f t="shared" si="0"/>
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>101</v>
@@ -14106,7 +14367,7 @@
       </c>
       <c r="C21" s="17">
         <f t="shared" si="0"/>
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>101</v>
@@ -14272,11 +14533,11 @@
       </c>
       <c r="B22" s="17">
         <f>mtl_newcases!C23</f>
-        <v>3646</v>
+        <v>3645</v>
       </c>
       <c r="C22" s="17">
         <f t="shared" si="0"/>
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>101</v>
@@ -14442,7 +14703,7 @@
       </c>
       <c r="B23" s="17">
         <f>mtl_newcases!C24</f>
-        <v>3907</v>
+        <v>3906</v>
       </c>
       <c r="C23" s="17">
         <f t="shared" si="0"/>
@@ -14612,11 +14873,11 @@
       </c>
       <c r="B24" s="17">
         <f>mtl_newcases!C25</f>
-        <v>4370</v>
+        <v>4368</v>
       </c>
       <c r="C24" s="17">
         <f t="shared" si="0"/>
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D24">
         <v>63</v>
@@ -14782,7 +15043,7 @@
       </c>
       <c r="B25" s="17">
         <f>mtl_newcases!C26</f>
-        <v>4792</v>
+        <v>4790</v>
       </c>
       <c r="C25" s="17">
         <f t="shared" si="0"/>
@@ -14953,11 +15214,11 @@
       </c>
       <c r="B26" s="17">
         <f>mtl_newcases!C27</f>
-        <v>5169</v>
+        <v>5168</v>
       </c>
       <c r="C26" s="17">
         <f t="shared" si="0"/>
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D26">
         <v>91</v>
@@ -15124,7 +15385,7 @@
       </c>
       <c r="B27" s="17">
         <f>mtl_newcases!C28</f>
-        <v>5521</v>
+        <v>5520</v>
       </c>
       <c r="C27" s="17">
         <f t="shared" si="0"/>
@@ -15295,7 +15556,7 @@
       </c>
       <c r="B28" s="17">
         <f>mtl_newcases!C29</f>
-        <v>5828</v>
+        <v>5827</v>
       </c>
       <c r="C28" s="17">
         <f t="shared" si="0"/>
@@ -15466,7 +15727,7 @@
       </c>
       <c r="B29" s="17">
         <f>mtl_newcases!C30</f>
-        <v>6090</v>
+        <v>6089</v>
       </c>
       <c r="C29" s="17">
         <f t="shared" si="0"/>
@@ -15637,11 +15898,11 @@
       </c>
       <c r="B30" s="17">
         <f>mtl_newcases!C31</f>
-        <v>6427</v>
+        <v>6424</v>
       </c>
       <c r="C30" s="17">
         <f t="shared" si="0"/>
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D30">
         <v>162</v>
@@ -15808,11 +16069,11 @@
       </c>
       <c r="B31" s="17">
         <f>mtl_newcases!C32</f>
-        <v>6968</v>
+        <v>6963</v>
       </c>
       <c r="C31" s="17">
         <f t="shared" si="0"/>
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D31">
         <v>218</v>
@@ -15979,7 +16240,7 @@
       </c>
       <c r="B32" s="17">
         <f>mtl_newcases!C33</f>
-        <v>7443</v>
+        <v>7438</v>
       </c>
       <c r="C32" s="17">
         <f t="shared" si="0"/>
@@ -16150,11 +16411,11 @@
       </c>
       <c r="B33" s="17">
         <f>mtl_newcases!C34</f>
-        <v>8075</v>
+        <v>8068</v>
       </c>
       <c r="C33" s="17">
         <f t="shared" si="0"/>
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D33">
         <v>332</v>
@@ -16321,11 +16582,11 @@
       </c>
       <c r="B34" s="17">
         <f>mtl_newcases!C35</f>
-        <v>8570</v>
+        <v>8562</v>
       </c>
       <c r="C34" s="17">
         <f t="shared" si="0"/>
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D34">
         <v>391</v>
@@ -16492,11 +16753,11 @@
       </c>
       <c r="B35" s="17">
         <f>mtl_newcases!C36</f>
-        <v>9145</v>
+        <v>9138</v>
       </c>
       <c r="C35" s="17">
         <f t="shared" si="0"/>
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D35">
         <v>454</v>
@@ -16663,11 +16924,11 @@
       </c>
       <c r="B36" s="17">
         <f>mtl_newcases!C37</f>
-        <v>9469</v>
+        <v>9460</v>
       </c>
       <c r="C36" s="17">
         <f t="shared" si="0"/>
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D36">
         <v>513</v>
@@ -16834,11 +17095,11 @@
       </c>
       <c r="B37" s="17">
         <f>mtl_newcases!C38</f>
-        <v>9900</v>
+        <v>9889</v>
       </c>
       <c r="C37" s="17">
         <f t="shared" si="0"/>
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D37">
         <v>525</v>
@@ -16974,11 +17235,11 @@
       </c>
       <c r="B38" s="17">
         <f>mtl_newcases!C39</f>
-        <v>10402</v>
+        <v>10388</v>
       </c>
       <c r="C38" s="17">
         <f t="shared" si="0"/>
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D38">
         <v>583</v>
@@ -17145,11 +17406,11 @@
       </c>
       <c r="B39" s="17">
         <f>mtl_newcases!C40</f>
-        <v>10880</v>
+        <v>10865</v>
       </c>
       <c r="C39" s="17">
         <f t="shared" si="0"/>
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D39">
         <v>647</v>
@@ -17316,11 +17577,11 @@
       </c>
       <c r="B40" s="17">
         <f>mtl_newcases!C41</f>
-        <v>11436</v>
+        <v>11418</v>
       </c>
       <c r="C40" s="17">
         <f t="shared" si="0"/>
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="D40">
         <v>741</v>
@@ -17487,11 +17748,11 @@
       </c>
       <c r="B41" s="17">
         <f>mtl_newcases!C42</f>
-        <v>11990</v>
+        <v>11967</v>
       </c>
       <c r="C41" s="17">
         <f t="shared" si="0"/>
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="D41">
         <v>808</v>
@@ -17658,11 +17919,11 @@
       </c>
       <c r="B42" s="17">
         <f>mtl_newcases!C43</f>
-        <v>12512</v>
+        <v>12479</v>
       </c>
       <c r="C42" s="17">
         <f t="shared" si="0"/>
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="D42">
         <v>895</v>
@@ -17829,11 +18090,11 @@
       </c>
       <c r="B43" s="17">
         <f>mtl_newcases!C44</f>
-        <v>12837</v>
+        <v>12803</v>
       </c>
       <c r="C43" s="17">
         <f t="shared" si="0"/>
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D43">
         <v>938</v>
@@ -18000,11 +18261,11 @@
       </c>
       <c r="B44" s="17">
         <f>mtl_newcases!C45</f>
-        <v>13154</v>
+        <v>13117</v>
       </c>
       <c r="C44" s="17">
         <f>B44-B43</f>
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D44">
         <v>983</v>
@@ -18171,11 +18432,11 @@
       </c>
       <c r="B45" s="17">
         <f>mtl_newcases!C46</f>
-        <v>13644</v>
+        <v>13601</v>
       </c>
       <c r="C45" s="17">
         <f>B45-B44</f>
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="D45">
         <v>1039</v>
@@ -18342,7 +18603,7 @@
       </c>
       <c r="B46" s="17">
         <f>mtl_newcases!C47</f>
-        <v>14121</v>
+        <v>14078</v>
       </c>
       <c r="C46" s="17">
         <f t="shared" ref="C46:C47" si="438">B46-B45</f>
@@ -18482,11 +18743,11 @@
       </c>
       <c r="B47" s="17">
         <f>mtl_newcases!C48</f>
-        <v>14652</v>
+        <v>14607</v>
       </c>
       <c r="C47" s="17">
         <f t="shared" si="438"/>
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D47">
         <v>1146</v>
@@ -18622,11 +18883,11 @@
       </c>
       <c r="B48" s="17">
         <f>mtl_newcases!C49</f>
-        <v>15256</v>
+        <v>15209</v>
       </c>
       <c r="C48" s="17">
         <f t="shared" ref="C48" si="439">B48-B47</f>
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D48">
         <v>1245</v>
@@ -18793,11 +19054,11 @@
       </c>
       <c r="B49" s="17">
         <f>mtl_newcases!C50</f>
-        <v>15883</v>
+        <v>15831</v>
       </c>
       <c r="C49" s="17">
         <f t="shared" ref="C49" si="461">B49-B48</f>
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="D49">
         <v>1312</v>
@@ -18964,11 +19225,11 @@
       </c>
       <c r="B50" s="17">
         <f>mtl_newcases!C51</f>
-        <v>16336</v>
+        <v>16317</v>
       </c>
       <c r="C50" s="17">
         <f t="shared" ref="C50" si="483">B50-B49</f>
-        <v>453</v>
+        <v>486</v>
       </c>
       <c r="D50">
         <v>1365</v>
@@ -19135,11 +19396,11 @@
       </c>
       <c r="B51" s="17">
         <f>mtl_newcases!C52</f>
-        <v>16687</v>
+        <v>16673</v>
       </c>
       <c r="C51" s="17">
         <f t="shared" ref="C51" si="505">B51-B50</f>
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="D51">
         <v>1410</v>
@@ -19310,7 +19571,7 @@
       </c>
       <c r="C52" s="17">
         <f t="shared" ref="C52" si="527">B52-B51</f>
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="D52">
         <v>1488</v>
@@ -19477,11 +19738,11 @@
       </c>
       <c r="B53" s="17">
         <f>mtl_newcases!C54</f>
-        <v>17573</v>
+        <v>17604</v>
       </c>
       <c r="C53" s="17">
         <f t="shared" ref="C53" si="549">B53-B52</f>
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="D53">
         <v>1562</v>
@@ -19648,11 +19909,11 @@
       </c>
       <c r="B54" s="17">
         <f>mtl_newcases!C55</f>
-        <v>17918</v>
+        <v>18138</v>
       </c>
       <c r="C54" s="17">
         <f t="shared" ref="C54:C55" si="571">B54-B53</f>
-        <v>345</v>
+        <v>534</v>
       </c>
       <c r="D54">
         <v>1666</v>
@@ -19823,7 +20084,7 @@
       </c>
       <c r="C55" s="17">
         <f t="shared" si="571"/>
-        <v>517</v>
+        <v>297</v>
       </c>
       <c r="D55">
         <v>1727</v>
@@ -19832,125 +20093,156 @@
         <f t="shared" si="572"/>
         <v>61</v>
       </c>
-      <c r="F55" t="s">
-        <v>101</v>
-      </c>
-      <c r="G55" t="s">
-        <v>101</v>
-      </c>
-      <c r="H55" t="s">
-        <v>101</v>
-      </c>
-      <c r="I55" t="s">
-        <v>101</v>
-      </c>
-      <c r="J55" t="s">
-        <v>101</v>
-      </c>
-      <c r="K55" t="s">
-        <v>101</v>
-      </c>
-      <c r="L55" t="s">
-        <v>101</v>
-      </c>
-      <c r="M55" t="s">
-        <v>101</v>
-      </c>
-      <c r="N55" t="s">
-        <v>101</v>
-      </c>
-      <c r="O55" t="s">
-        <v>101</v>
-      </c>
-      <c r="P55" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>101</v>
-      </c>
-      <c r="R55" t="s">
-        <v>101</v>
-      </c>
-      <c r="S55" t="s">
-        <v>101</v>
-      </c>
-      <c r="T55" t="s">
-        <v>101</v>
-      </c>
-      <c r="U55" t="s">
-        <v>101</v>
-      </c>
-      <c r="V55" t="s">
-        <v>101</v>
-      </c>
-      <c r="W55" t="s">
-        <v>101</v>
-      </c>
-      <c r="X55" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y55" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AD55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AF55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AG55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AH55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AI55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AJ55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AK55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AL55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AM55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AN55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AO55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AP55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AQ55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AR55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AS55" t="s">
-        <v>101</v>
+      <c r="F55" cm="1">
+        <f t="array" ref="F55:O55">TRANSPOSE(santemontreal!AN$57:AN$66)</f>
+        <v>175</v>
+      </c>
+      <c r="G55">
+        <v>144</v>
+      </c>
+      <c r="H55">
+        <v>528</v>
+      </c>
+      <c r="I55">
+        <v>1943</v>
+      </c>
+      <c r="J55">
+        <v>2235</v>
+      </c>
+      <c r="K55">
+        <v>2545</v>
+      </c>
+      <c r="L55">
+        <v>2342</v>
+      </c>
+      <c r="M55">
+        <v>1622</v>
+      </c>
+      <c r="N55">
+        <v>1764</v>
+      </c>
+      <c r="O55">
+        <v>5068</v>
+      </c>
+      <c r="P55" s="18">
+        <f>F55/(age_distribution_2016!$B$2/100000)</f>
+        <v>159.46783305995993</v>
+      </c>
+      <c r="Q55" s="18">
+        <f>G55/(age_distribution_2016!$B$3/100000)</f>
+        <v>137.95085500790344</v>
+      </c>
+      <c r="R55" s="18">
+        <f>H55/(age_distribution_2016!$B$4/100000)</f>
+        <v>280.57496612376121</v>
+      </c>
+      <c r="S55" s="18">
+        <f>I55/(age_distribution_2016!$B$5/100000)</f>
+        <v>662.6310853440192</v>
+      </c>
+      <c r="T55" s="18">
+        <f>J55/(age_distribution_2016!$B$6/100000)</f>
+        <v>745.80795862184027</v>
+      </c>
+      <c r="U55" s="18">
+        <f>K55/(age_distribution_2016!$B$7/100000)</f>
+        <v>1000.0982414775518</v>
+      </c>
+      <c r="V55" s="18">
+        <f>L55/(age_distribution_2016!$B$8/100000)</f>
+        <v>904.68372766779328</v>
+      </c>
+      <c r="W55" s="18">
+        <f>M55/(age_distribution_2016!$B$9/100000)</f>
+        <v>791.20021462891145</v>
+      </c>
+      <c r="X55" s="18">
+        <f>N55/(age_distribution_2016!$B$10/100000)</f>
+        <v>1360.2714373843307</v>
+      </c>
+      <c r="Y55" s="18">
+        <f>O55/(age_distribution_2016!$B$11/100000)</f>
+        <v>5129.2950761601132</v>
+      </c>
+      <c r="Z55" s="3">
+        <f t="shared" ref="Z55" si="593">F55*100/SUM($F55:$O55)</f>
+        <v>0.9528476532723511</v>
+      </c>
+      <c r="AA55" s="3">
+        <f t="shared" ref="AA55" si="594">G55*100/SUM($F55:$O55)</f>
+        <v>0.78405749754982035</v>
+      </c>
+      <c r="AB55" s="3">
+        <f t="shared" ref="AB55" si="595">H55*100/SUM($F55:$O55)</f>
+        <v>2.874877491016008</v>
+      </c>
+      <c r="AC55" s="3">
+        <f t="shared" ref="AC55" si="596">I55*100/SUM($F55:$O55)</f>
+        <v>10.579331373189589</v>
+      </c>
+      <c r="AD55" s="3">
+        <f t="shared" ref="AD55" si="597">J55*100/SUM($F55:$O55)</f>
+        <v>12.169225743221169</v>
+      </c>
+      <c r="AE55" s="3">
+        <f t="shared" ref="AE55" si="598">K55*100/SUM($F55:$O55)</f>
+        <v>13.857127300446477</v>
+      </c>
+      <c r="AF55" s="3">
+        <f t="shared" ref="AF55" si="599">L55*100/SUM($F55:$O55)</f>
+        <v>12.751824022650551</v>
+      </c>
+      <c r="AG55" s="3">
+        <f t="shared" ref="AG55" si="600">M55*100/SUM($F55:$O55)</f>
+        <v>8.8315365349014492</v>
+      </c>
+      <c r="AH55" s="3">
+        <f t="shared" ref="AH55" si="601">N55*100/SUM($F55:$O55)</f>
+        <v>9.6047043449852989</v>
+      </c>
+      <c r="AI55" s="3">
+        <f t="shared" ref="AI55" si="602">O55*100/SUM($F55:$O55)</f>
+        <v>27.594468038767289</v>
+      </c>
+      <c r="AJ55" s="3">
+        <f t="shared" ref="AJ55" si="603">P55*100/SUM($P55:$Y55)</f>
+        <v>1.4273907860653299</v>
+      </c>
+      <c r="AK55" s="3">
+        <f t="shared" ref="AK55" si="604">Q55*100/SUM($P55:$Y55)</f>
+        <v>1.2347930964489719</v>
+      </c>
+      <c r="AL55" s="3">
+        <f t="shared" ref="AL55" si="605">R55*100/SUM($P55:$Y55)</f>
+        <v>2.5114163387111712</v>
+      </c>
+      <c r="AM55" s="3">
+        <f t="shared" ref="AM55" si="606">S55*100/SUM($P55:$Y55)</f>
+        <v>5.9311867956773998</v>
+      </c>
+      <c r="AN55" s="3">
+        <f t="shared" ref="AN55" si="607">T55*100/SUM($P55:$Y55)</f>
+        <v>6.6756999696028547</v>
+      </c>
+      <c r="AO55" s="3">
+        <f t="shared" ref="AO55" si="608">U55*100/SUM($P55:$Y55)</f>
+        <v>8.9518430623462777</v>
+      </c>
+      <c r="AP55" s="3">
+        <f t="shared" ref="AP55" si="609">V55*100/SUM($P55:$Y55)</f>
+        <v>8.097791212166916</v>
+      </c>
+      <c r="AQ55" s="3">
+        <f t="shared" ref="AQ55" si="610">W55*100/SUM($P55:$Y55)</f>
+        <v>7.0820044056758658</v>
+      </c>
+      <c r="AR55" s="3">
+        <f t="shared" ref="AR55" si="611">X55*100/SUM($P55:$Y55)</f>
+        <v>12.17574026694261</v>
+      </c>
+      <c r="AS55" s="3">
+        <f t="shared" ref="AS55" si="612">Y55*100/SUM($P55:$Y55)</f>
+        <v>45.912134066362597</v>
       </c>
     </row>
   </sheetData>
@@ -22529,8 +22821,8 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22809,11 +23101,11 @@
         <v>43922</v>
       </c>
       <c r="B20">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="E20" s="19">
         <v>43922</v>
@@ -22823,7 +23115,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>-83</v>
+        <v>-84</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -22831,11 +23123,11 @@
         <v>43923</v>
       </c>
       <c r="B21">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>2956</v>
+        <v>2954</v>
       </c>
       <c r="E21" s="19">
         <v>43923</v>
@@ -22845,7 +23137,7 @@
       </c>
       <c r="G21">
         <f t="shared" ref="G21:G26" si="2">C21-F21</f>
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -22853,7 +23145,7 @@
         <v>43924</v>
       </c>
       <c r="B22">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
@@ -22875,11 +23167,11 @@
         <v>43925</v>
       </c>
       <c r="B23">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>3646</v>
+        <v>3645</v>
       </c>
       <c r="E23" s="19">
         <v>43925</v>
@@ -22889,7 +23181,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>-67</v>
+        <v>-68</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -22901,7 +23193,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>3907</v>
+        <v>3906</v>
       </c>
       <c r="E24" s="19">
         <v>43926</v>
@@ -22911,7 +23203,7 @@
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>-70</v>
+        <v>-71</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -22919,11 +23211,11 @@
         <v>43927</v>
       </c>
       <c r="B25">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>4370</v>
+        <v>4368</v>
       </c>
       <c r="E25" s="19">
         <v>43927</v>
@@ -22933,7 +23225,7 @@
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>-37</v>
+        <v>-39</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -22945,7 +23237,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>4792</v>
+        <v>4790</v>
       </c>
       <c r="E26" s="19">
         <v>43928</v>
@@ -22955,7 +23247,7 @@
       </c>
       <c r="G26">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -22963,11 +23255,11 @@
         <v>43929</v>
       </c>
       <c r="B27">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>5169</v>
+        <v>5168</v>
       </c>
       <c r="E27" s="19">
         <v>43929</v>
@@ -22977,7 +23269,7 @@
       </c>
       <c r="G27">
         <f t="shared" ref="G27" si="3">C27-F27</f>
-        <v>-93</v>
+        <v>-94</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -22989,7 +23281,7 @@
       </c>
       <c r="C28">
         <f t="shared" ref="C28:C37" si="4">C27+B28</f>
-        <v>5521</v>
+        <v>5520</v>
       </c>
       <c r="E28" s="19">
         <v>43930</v>
@@ -22999,7 +23291,7 @@
       </c>
       <c r="G28">
         <f t="shared" ref="G28:G33" si="5">C28-F28</f>
-        <v>-96</v>
+        <v>-97</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -23011,7 +23303,7 @@
       </c>
       <c r="C29">
         <f t="shared" si="4"/>
-        <v>5828</v>
+        <v>5827</v>
       </c>
       <c r="E29" s="19">
         <v>43931</v>
@@ -23021,7 +23313,7 @@
       </c>
       <c r="G29">
         <f t="shared" si="5"/>
-        <v>-33</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -23033,7 +23325,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="4"/>
-        <v>6090</v>
+        <v>6089</v>
       </c>
       <c r="E30" s="19">
         <v>43932</v>
@@ -23043,7 +23335,7 @@
       </c>
       <c r="G30">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -23051,11 +23343,11 @@
         <v>43933</v>
       </c>
       <c r="B31">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C31">
         <f t="shared" si="4"/>
-        <v>6427</v>
+        <v>6424</v>
       </c>
       <c r="E31" s="19">
         <v>43933</v>
@@ -23065,7 +23357,7 @@
       </c>
       <c r="G31">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -23073,11 +23365,11 @@
         <v>43934</v>
       </c>
       <c r="B32">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C32">
         <f t="shared" si="4"/>
-        <v>6968</v>
+        <v>6963</v>
       </c>
       <c r="E32" s="19">
         <v>43934</v>
@@ -23087,7 +23379,7 @@
       </c>
       <c r="G32">
         <f t="shared" si="5"/>
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -23099,7 +23391,7 @@
       </c>
       <c r="C33">
         <f t="shared" si="4"/>
-        <v>7443</v>
+        <v>7438</v>
       </c>
       <c r="E33" s="19">
         <v>43935</v>
@@ -23109,7 +23401,7 @@
       </c>
       <c r="G33">
         <f t="shared" si="5"/>
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -23117,11 +23409,11 @@
         <v>43936</v>
       </c>
       <c r="B34">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C34">
         <f t="shared" si="4"/>
-        <v>8075</v>
+        <v>8068</v>
       </c>
       <c r="E34" s="19">
         <v>43936</v>
@@ -23131,7 +23423,7 @@
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G36" si="6">C34-F34</f>
-        <v>794</v>
+        <v>787</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -23139,11 +23431,11 @@
         <v>43937</v>
       </c>
       <c r="B35">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C35">
         <f t="shared" si="4"/>
-        <v>8570</v>
+        <v>8562</v>
       </c>
       <c r="E35" s="19">
         <v>43937</v>
@@ -23153,7 +23445,7 @@
       </c>
       <c r="G35">
         <f t="shared" si="6"/>
-        <v>810</v>
+        <v>802</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -23161,11 +23453,11 @@
         <v>43938</v>
       </c>
       <c r="B36">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C36">
         <f t="shared" si="4"/>
-        <v>9145</v>
+        <v>9138</v>
       </c>
       <c r="E36" s="19">
         <v>43938</v>
@@ -23175,7 +23467,7 @@
       </c>
       <c r="G36">
         <f t="shared" si="6"/>
-        <v>1093</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -23183,11 +23475,11 @@
         <v>43939</v>
       </c>
       <c r="B37" s="23">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C37">
         <f t="shared" si="4"/>
-        <v>9469</v>
+        <v>9460</v>
       </c>
       <c r="E37" s="19">
         <v>43939</v>
@@ -23197,7 +23489,7 @@
       </c>
       <c r="G37">
         <f t="shared" ref="G37" si="7">C37-F37</f>
-        <v>1012</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -23205,11 +23497,11 @@
         <v>43940</v>
       </c>
       <c r="B38" s="23">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C38">
         <f t="shared" ref="C38:C39" si="8">C37+B38</f>
-        <v>9900</v>
+        <v>9889</v>
       </c>
       <c r="E38" s="19">
         <v>43940</v>
@@ -23219,7 +23511,7 @@
       </c>
       <c r="G38">
         <f t="shared" ref="G38" si="9">C38-F38</f>
-        <v>936</v>
+        <v>925</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -23227,11 +23519,11 @@
         <v>43941</v>
       </c>
       <c r="B39">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C39">
         <f t="shared" si="8"/>
-        <v>10402</v>
+        <v>10388</v>
       </c>
       <c r="E39" s="19">
         <v>43941</v>
@@ -23241,7 +23533,7 @@
       </c>
       <c r="G39">
         <f t="shared" ref="G39" si="10">C39-F39</f>
-        <v>1054</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -23249,11 +23541,11 @@
         <v>43942</v>
       </c>
       <c r="B40">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C40">
         <f t="shared" ref="C40" si="11">C39+B40</f>
-        <v>10880</v>
+        <v>10865</v>
       </c>
       <c r="E40" s="19">
         <v>43942</v>
@@ -23263,7 +23555,7 @@
       </c>
       <c r="G40">
         <f t="shared" ref="G40" si="12">C40-F40</f>
-        <v>1024</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -23271,11 +23563,11 @@
         <v>43943</v>
       </c>
       <c r="B41">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C41">
         <f t="shared" ref="C41:C52" si="13">C40+B41</f>
-        <v>11436</v>
+        <v>11418</v>
       </c>
       <c r="E41" s="19">
         <v>43943</v>
@@ -23285,7 +23577,7 @@
       </c>
       <c r="G41">
         <f t="shared" ref="G41" si="14">C41-F41</f>
-        <v>1061</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -23293,11 +23585,11 @@
         <v>43944</v>
       </c>
       <c r="B42" s="23">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C42">
         <f t="shared" si="13"/>
-        <v>11990</v>
+        <v>11967</v>
       </c>
       <c r="E42" s="19">
         <v>43944</v>
@@ -23307,7 +23599,7 @@
       </c>
       <c r="G42">
         <f t="shared" ref="G42:G44" si="15">C42-F42</f>
-        <v>1093</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -23315,11 +23607,11 @@
         <v>43945</v>
       </c>
       <c r="B43" s="23">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="C43">
         <f t="shared" si="13"/>
-        <v>12512</v>
+        <v>12479</v>
       </c>
       <c r="E43" s="19">
         <v>43945</v>
@@ -23329,7 +23621,7 @@
       </c>
       <c r="G43">
         <f t="shared" si="15"/>
-        <v>1351</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -23337,11 +23629,11 @@
         <v>43946</v>
       </c>
       <c r="B44" s="23">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C44">
         <f t="shared" si="13"/>
-        <v>12837</v>
+        <v>12803</v>
       </c>
       <c r="E44" s="19">
         <v>43946</v>
@@ -23351,7 +23643,7 @@
       </c>
       <c r="G44">
         <f t="shared" si="15"/>
-        <v>1216</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -23359,11 +23651,11 @@
         <v>43947</v>
       </c>
       <c r="B45" s="23">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C45">
         <f t="shared" si="13"/>
-        <v>13154</v>
+        <v>13117</v>
       </c>
       <c r="E45" s="19">
         <v>43947</v>
@@ -23373,7 +23665,7 @@
       </c>
       <c r="G45">
         <f>C45-F45</f>
-        <v>1120</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -23381,11 +23673,11 @@
         <v>43948</v>
       </c>
       <c r="B46" s="23">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="C46">
         <f t="shared" si="13"/>
-        <v>13644</v>
+        <v>13601</v>
       </c>
       <c r="E46" s="19">
         <v>43948</v>
@@ -23395,7 +23687,7 @@
       </c>
       <c r="G46">
         <f>C46-F46</f>
-        <v>1157</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -23407,7 +23699,7 @@
       </c>
       <c r="C47">
         <f t="shared" si="13"/>
-        <v>14121</v>
+        <v>14078</v>
       </c>
       <c r="E47" s="19">
         <v>43949</v>
@@ -23417,7 +23709,7 @@
       </c>
       <c r="G47">
         <f t="shared" ref="G47:G52" si="16">C47-F47</f>
-        <v>1310</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -23425,11 +23717,11 @@
         <v>43950</v>
       </c>
       <c r="B48" s="23">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C48">
         <f t="shared" si="13"/>
-        <v>14652</v>
+        <v>14607</v>
       </c>
       <c r="E48" s="19">
         <v>43950</v>
@@ -23439,7 +23731,7 @@
       </c>
       <c r="G48">
         <f t="shared" si="16"/>
-        <v>1328</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -23447,11 +23739,11 @@
         <v>43951</v>
       </c>
       <c r="B49" s="23">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C49">
         <f t="shared" si="13"/>
-        <v>15256</v>
+        <v>15209</v>
       </c>
       <c r="E49" s="19">
         <v>43951</v>
@@ -23461,7 +23753,7 @@
       </c>
       <c r="G49">
         <f t="shared" si="16"/>
-        <v>1277</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -23469,11 +23761,11 @@
         <v>43952</v>
       </c>
       <c r="B50" s="23">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="C50">
         <f t="shared" si="13"/>
-        <v>15883</v>
+        <v>15831</v>
       </c>
       <c r="E50" s="19">
         <v>43952</v>
@@ -23483,7 +23775,7 @@
       </c>
       <c r="G50">
         <f t="shared" si="16"/>
-        <v>1284</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -23491,11 +23783,11 @@
         <v>43953</v>
       </c>
       <c r="B51" s="23">
-        <v>453</v>
+        <v>486</v>
       </c>
       <c r="C51">
         <f t="shared" si="13"/>
-        <v>16336</v>
+        <v>16317</v>
       </c>
       <c r="E51" s="19">
         <v>43953</v>
@@ -23505,7 +23797,7 @@
       </c>
       <c r="G51">
         <f t="shared" si="16"/>
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -23513,11 +23805,11 @@
         <v>43954</v>
       </c>
       <c r="B52" s="23">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="C52">
         <f t="shared" si="13"/>
-        <v>16687</v>
+        <v>16673</v>
       </c>
       <c r="E52" s="19">
         <v>43954</v>
@@ -23527,7 +23819,7 @@
       </c>
       <c r="G52">
         <f t="shared" si="16"/>
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -23535,7 +23827,7 @@
         <v>43955</v>
       </c>
       <c r="B53" s="23">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="C53">
         <f t="shared" ref="C53" si="17">C52+B53</f>
@@ -23557,11 +23849,11 @@
         <v>43956</v>
       </c>
       <c r="B54" s="23">
-        <v>485</v>
+        <v>516</v>
       </c>
       <c r="C54">
         <f t="shared" ref="C54:C56" si="19">C53+B54</f>
-        <v>17573</v>
+        <v>17604</v>
       </c>
       <c r="E54" s="19">
         <v>43956</v>
@@ -23571,19 +23863,19 @@
       </c>
       <c r="G54">
         <f t="shared" ref="G54" si="20">C54-F54</f>
-        <v>131</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="19">
         <v>43957</v>
       </c>
-      <c r="B55" s="24">
-        <v>345</v>
+      <c r="B55" s="23">
+        <v>534</v>
       </c>
       <c r="C55">
         <f t="shared" si="19"/>
-        <v>17918</v>
+        <v>18138</v>
       </c>
       <c r="E55" s="19">
         <v>43957</v>
@@ -23593,7 +23885,7 @@
       </c>
       <c r="G55">
         <f t="shared" ref="G55:G56" si="21">C55-F55</f>
-        <v>0</v>
+        <v>220</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -23601,7 +23893,7 @@
         <v>43958</v>
       </c>
       <c r="B56" s="24">
-        <v>517</v>
+        <v>297</v>
       </c>
       <c r="C56">
         <f t="shared" si="19"/>
@@ -23628,9 +23920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E261AEA-18EA-4FE9-ACAC-1FB61BEBD535}">
   <dimension ref="A1:HH119"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM2" sqref="AM2:AM36"/>
+      <selection pane="topRight" activeCell="AN35" sqref="AN2:AN35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23757,9 +24049,11 @@
         <v>300</v>
       </c>
       <c r="AM1" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="AN1" s="5"/>
+        <v>304</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>310</v>
+      </c>
       <c r="AO1" s="5"/>
       <c r="AP1" s="5"/>
       <c r="AQ1" s="5"/>
@@ -24055,7 +24349,9 @@
       <c r="AM2" s="7">
         <v>1442</v>
       </c>
-      <c r="AN2" s="7"/>
+      <c r="AN2" s="7">
+        <v>1502</v>
+      </c>
       <c r="AO2" s="7"/>
       <c r="AP2" s="7"/>
       <c r="AQ2" s="7"/>
@@ -24351,7 +24647,9 @@
       <c r="AM3" s="9">
         <v>398</v>
       </c>
-      <c r="AN3" s="9"/>
+      <c r="AN3" s="9">
+        <v>409</v>
+      </c>
       <c r="AO3" s="9"/>
       <c r="AP3" s="9"/>
       <c r="AQ3" s="9"/>
@@ -24647,7 +24945,9 @@
       <c r="AM4" s="7">
         <v>10</v>
       </c>
-      <c r="AN4" s="7"/>
+      <c r="AN4" s="7">
+        <v>11</v>
+      </c>
       <c r="AO4" s="7"/>
       <c r="AP4" s="7"/>
       <c r="AQ4" s="7"/>
@@ -24943,7 +25243,9 @@
       <c r="AM5" s="9">
         <v>46</v>
       </c>
-      <c r="AN5" s="9"/>
+      <c r="AN5" s="9">
+        <v>45</v>
+      </c>
       <c r="AO5" s="9"/>
       <c r="AP5" s="9"/>
       <c r="AQ5" s="9"/>
@@ -25239,7 +25541,9 @@
       <c r="AM6" s="7">
         <v>1478</v>
       </c>
-      <c r="AN6" s="7"/>
+      <c r="AN6" s="7">
+        <v>1512</v>
+      </c>
       <c r="AO6" s="7"/>
       <c r="AP6" s="7"/>
       <c r="AQ6" s="7"/>
@@ -25535,7 +25839,9 @@
       <c r="AM7" s="9">
         <v>390</v>
       </c>
-      <c r="AN7" s="9"/>
+      <c r="AN7" s="9">
+        <v>393</v>
+      </c>
       <c r="AO7" s="9"/>
       <c r="AP7" s="9"/>
       <c r="AQ7" s="9"/>
@@ -25831,7 +26137,9 @@
       <c r="AM8" s="7">
         <v>271</v>
       </c>
-      <c r="AN8" s="7"/>
+      <c r="AN8" s="7">
+        <v>274</v>
+      </c>
       <c r="AO8" s="7"/>
       <c r="AP8" s="7"/>
       <c r="AQ8" s="7"/>
@@ -26127,7 +26435,9 @@
       <c r="AM9" s="9">
         <v>137</v>
       </c>
-      <c r="AN9" s="9"/>
+      <c r="AN9" s="9">
+        <v>141</v>
+      </c>
       <c r="AO9" s="9"/>
       <c r="AP9" s="9"/>
       <c r="AQ9" s="9"/>
@@ -26423,7 +26733,9 @@
       <c r="AM10" s="7">
         <v>42</v>
       </c>
-      <c r="AN10" s="7"/>
+      <c r="AN10" s="7">
+        <v>42</v>
+      </c>
       <c r="AO10" s="7"/>
       <c r="AP10" s="7"/>
       <c r="AQ10" s="7"/>
@@ -26719,7 +27031,9 @@
       <c r="AM11" s="9">
         <v>77</v>
       </c>
-      <c r="AN11" s="9"/>
+      <c r="AN11" s="9">
+        <v>77</v>
+      </c>
       <c r="AO11" s="9"/>
       <c r="AP11" s="9"/>
       <c r="AQ11" s="9"/>
@@ -27015,7 +27329,9 @@
       <c r="AM12" s="7">
         <v>378</v>
       </c>
-      <c r="AN12" s="7"/>
+      <c r="AN12" s="7">
+        <v>386</v>
+      </c>
       <c r="AO12" s="7"/>
       <c r="AP12" s="7"/>
       <c r="AQ12" s="7"/>
@@ -27311,7 +27627,9 @@
       <c r="AM13" s="9">
         <v>888</v>
       </c>
-      <c r="AN13" s="9"/>
+      <c r="AN13" s="9">
+        <v>902</v>
+      </c>
       <c r="AO13" s="9"/>
       <c r="AP13" s="9"/>
       <c r="AQ13" s="9"/>
@@ -27607,7 +27925,9 @@
       <c r="AM14" s="7">
         <v>118</v>
       </c>
-      <c r="AN14" s="7"/>
+      <c r="AN14" s="7">
+        <v>125</v>
+      </c>
       <c r="AO14" s="7"/>
       <c r="AP14" s="7"/>
       <c r="AQ14" s="7"/>
@@ -27903,7 +28223,9 @@
       <c r="AM15" s="9">
         <v>1341</v>
       </c>
-      <c r="AN15" s="9"/>
+      <c r="AN15" s="9">
+        <v>1402</v>
+      </c>
       <c r="AO15" s="9"/>
       <c r="AP15" s="9"/>
       <c r="AQ15" s="9"/>
@@ -28199,7 +28521,9 @@
       <c r="AM16" s="7">
         <v>24</v>
       </c>
-      <c r="AN16" s="7"/>
+      <c r="AN16" s="7">
+        <v>24</v>
+      </c>
       <c r="AO16" s="7"/>
       <c r="AP16" s="7"/>
       <c r="AQ16" s="7"/>
@@ -28495,7 +28819,9 @@
       <c r="AM17" s="9">
         <v>1615</v>
       </c>
-      <c r="AN17" s="9"/>
+      <c r="AN17" s="9">
+        <v>1676</v>
+      </c>
       <c r="AO17" s="9"/>
       <c r="AP17" s="9"/>
       <c r="AQ17" s="9"/>
@@ -28791,7 +29117,9 @@
       <c r="AM18" s="7">
         <v>14</v>
       </c>
-      <c r="AN18" s="7"/>
+      <c r="AN18" s="7">
+        <v>15</v>
+      </c>
       <c r="AO18" s="7"/>
       <c r="AP18" s="7"/>
       <c r="AQ18" s="7"/>
@@ -29087,7 +29415,9 @@
       <c r="AM19" s="9">
         <v>202</v>
       </c>
-      <c r="AN19" s="9"/>
+      <c r="AN19" s="9">
+        <v>207</v>
+      </c>
       <c r="AO19" s="9"/>
       <c r="AP19" s="9"/>
       <c r="AQ19" s="9"/>
@@ -29383,7 +29713,9 @@
       <c r="AM20" s="7">
         <v>215</v>
       </c>
-      <c r="AN20" s="7"/>
+      <c r="AN20" s="7">
+        <v>217</v>
+      </c>
       <c r="AO20" s="7"/>
       <c r="AP20" s="7"/>
       <c r="AQ20" s="7"/>
@@ -29679,7 +30011,9 @@
       <c r="AM21" s="9">
         <v>324</v>
       </c>
-      <c r="AN21" s="9"/>
+      <c r="AN21" s="9">
+        <v>337</v>
+      </c>
       <c r="AO21" s="9"/>
       <c r="AP21" s="9"/>
       <c r="AQ21" s="9"/>
@@ -29975,7 +30309,9 @@
       <c r="AM22" s="7">
         <v>649</v>
       </c>
-      <c r="AN22" s="7"/>
+      <c r="AN22" s="7">
+        <v>657</v>
+      </c>
       <c r="AO22" s="7"/>
       <c r="AP22" s="7"/>
       <c r="AQ22" s="7"/>
@@ -30271,7 +30607,9 @@
       <c r="AM23" s="9">
         <v>142</v>
       </c>
-      <c r="AN23" s="9"/>
+      <c r="AN23" s="9">
+        <v>142</v>
+      </c>
       <c r="AO23" s="9"/>
       <c r="AP23" s="9"/>
       <c r="AQ23" s="9"/>
@@ -30567,7 +30905,9 @@
       <c r="AM24" s="7">
         <v>1300</v>
       </c>
-      <c r="AN24" s="7"/>
+      <c r="AN24" s="7">
+        <v>1361</v>
+      </c>
       <c r="AO24" s="7"/>
       <c r="AP24" s="7"/>
       <c r="AQ24" s="7"/>
@@ -30863,7 +31203,9 @@
       <c r="AM25" s="9">
         <v>978</v>
       </c>
-      <c r="AN25" s="9"/>
+      <c r="AN25" s="9">
+        <v>1016</v>
+      </c>
       <c r="AO25" s="9"/>
       <c r="AP25" s="9"/>
       <c r="AQ25" s="9"/>
@@ -31159,7 +31501,9 @@
       <c r="AM26" s="7">
         <v>16</v>
       </c>
-      <c r="AN26" s="7"/>
+      <c r="AN26" s="7">
+        <v>15</v>
+      </c>
       <c r="AO26" s="7"/>
       <c r="AP26" s="7"/>
       <c r="AQ26" s="7"/>
@@ -31455,7 +31799,9 @@
       <c r="AM27" s="9">
         <v>645</v>
       </c>
-      <c r="AN27" s="9"/>
+      <c r="AN27" s="9">
+        <v>654</v>
+      </c>
       <c r="AO27" s="9"/>
       <c r="AP27" s="9"/>
       <c r="AQ27" s="9"/>
@@ -31751,7 +32097,9 @@
       <c r="AM28" s="7">
         <v>694</v>
       </c>
-      <c r="AN28" s="7"/>
+      <c r="AN28" s="7">
+        <v>716</v>
+      </c>
       <c r="AO28" s="7"/>
       <c r="AP28" s="7"/>
       <c r="AQ28" s="7"/>
@@ -32047,7 +32395,9 @@
       <c r="AM29" s="20">
         <v>2</v>
       </c>
-      <c r="AN29" s="22"/>
+      <c r="AN29" s="20">
+        <v>2</v>
+      </c>
       <c r="AO29" s="22"/>
       <c r="AP29" s="22"/>
       <c r="AQ29" s="22"/>
@@ -32343,7 +32693,9 @@
       <c r="AM30" s="7">
         <v>694</v>
       </c>
-      <c r="AN30" s="7"/>
+      <c r="AN30" s="7">
+        <v>708</v>
+      </c>
       <c r="AO30" s="7"/>
       <c r="AP30" s="7"/>
       <c r="AQ30" s="7"/>
@@ -32639,7 +32991,9 @@
       <c r="AM31" s="9">
         <v>738</v>
       </c>
-      <c r="AN31" s="9"/>
+      <c r="AN31" s="9">
+        <v>746</v>
+      </c>
       <c r="AO31" s="9"/>
       <c r="AP31" s="9"/>
       <c r="AQ31" s="9"/>
@@ -32935,7 +33289,9 @@
       <c r="AM32" s="7">
         <v>475</v>
       </c>
-      <c r="AN32" s="7"/>
+      <c r="AN32" s="7">
+        <v>495</v>
+      </c>
       <c r="AO32" s="7"/>
       <c r="AP32" s="7"/>
       <c r="AQ32" s="7"/>
@@ -33231,7 +33587,9 @@
       <c r="AM33" s="9">
         <v>1268</v>
       </c>
-      <c r="AN33" s="9"/>
+      <c r="AN33" s="9">
+        <v>1307</v>
+      </c>
       <c r="AO33" s="9"/>
       <c r="AP33" s="9"/>
       <c r="AQ33" s="9"/>
@@ -33527,7 +33885,9 @@
       <c r="AM34" s="7">
         <v>143</v>
       </c>
-      <c r="AN34" s="7"/>
+      <c r="AN34" s="7">
+        <v>143</v>
+      </c>
       <c r="AO34" s="7"/>
       <c r="AP34" s="7"/>
       <c r="AQ34" s="7"/>
@@ -33823,7 +34183,9 @@
       <c r="AM35" s="9">
         <v>765</v>
       </c>
-      <c r="AN35" s="9"/>
+      <c r="AN35" s="9">
+        <v>777</v>
+      </c>
       <c r="AO35" s="9"/>
       <c r="AP35" s="9"/>
       <c r="AQ35" s="9"/>
@@ -34119,7 +34481,9 @@
       <c r="AM36" s="11">
         <v>17918</v>
       </c>
-      <c r="AN36" s="11"/>
+      <c r="AN36" s="11">
+        <v>18435</v>
+      </c>
       <c r="AO36" s="11"/>
       <c r="AP36" s="11"/>
       <c r="AQ36" s="11"/>
@@ -38570,7 +38934,9 @@
       <c r="AM57" s="7">
         <v>167</v>
       </c>
-      <c r="AN57" s="7"/>
+      <c r="AN57" s="7">
+        <v>175</v>
+      </c>
       <c r="AO57" s="7"/>
       <c r="AP57" s="7"/>
       <c r="AQ57" s="7"/>
@@ -38864,7 +39230,9 @@
       <c r="AM58" s="9">
         <v>140</v>
       </c>
-      <c r="AN58" s="9"/>
+      <c r="AN58" s="9">
+        <v>144</v>
+      </c>
       <c r="AO58" s="9"/>
       <c r="AP58" s="9"/>
       <c r="AQ58" s="9"/>
@@ -39158,7 +39526,9 @@
       <c r="AM59" s="7">
         <v>512</v>
       </c>
-      <c r="AN59" s="7"/>
+      <c r="AN59" s="7">
+        <v>528</v>
+      </c>
       <c r="AO59" s="7"/>
       <c r="AP59" s="7"/>
       <c r="AQ59" s="7"/>
@@ -39452,7 +39822,9 @@
       <c r="AM60" s="9">
         <v>1893</v>
       </c>
-      <c r="AN60" s="9"/>
+      <c r="AN60" s="9">
+        <v>1943</v>
+      </c>
       <c r="AO60" s="9"/>
       <c r="AP60" s="9"/>
       <c r="AQ60" s="9"/>
@@ -39746,7 +40118,9 @@
       <c r="AM61" s="7">
         <v>2169</v>
       </c>
-      <c r="AN61" s="7"/>
+      <c r="AN61" s="7">
+        <v>2235</v>
+      </c>
       <c r="AO61" s="7"/>
       <c r="AP61" s="7"/>
       <c r="AQ61" s="7"/>
@@ -40040,7 +40414,9 @@
       <c r="AM62" s="9">
         <v>2485</v>
       </c>
-      <c r="AN62" s="9"/>
+      <c r="AN62" s="9">
+        <v>2545</v>
+      </c>
       <c r="AO62" s="9"/>
       <c r="AP62" s="9"/>
       <c r="AQ62" s="9"/>
@@ -40334,7 +40710,9 @@
       <c r="AM63" s="7">
         <v>2272</v>
       </c>
-      <c r="AN63" s="7"/>
+      <c r="AN63" s="7">
+        <v>2342</v>
+      </c>
       <c r="AO63" s="7"/>
       <c r="AP63" s="7"/>
       <c r="AQ63" s="7"/>
@@ -40628,7 +41006,9 @@
       <c r="AM64" s="9">
         <v>1572</v>
       </c>
-      <c r="AN64" s="9"/>
+      <c r="AN64" s="9">
+        <v>1622</v>
+      </c>
       <c r="AO64" s="9"/>
       <c r="AP64" s="9"/>
       <c r="AQ64" s="9"/>
@@ -40922,7 +41302,9 @@
       <c r="AM65" s="7">
         <v>1711</v>
       </c>
-      <c r="AN65" s="7"/>
+      <c r="AN65" s="7">
+        <v>1764</v>
+      </c>
       <c r="AO65" s="7"/>
       <c r="AP65" s="7"/>
       <c r="AQ65" s="7"/>
@@ -41216,7 +41598,9 @@
       <c r="AM66" s="9">
         <v>4929</v>
       </c>
-      <c r="AN66" s="9"/>
+      <c r="AN66" s="9">
+        <v>5068</v>
+      </c>
       <c r="AO66" s="9"/>
       <c r="AP66" s="9"/>
       <c r="AQ66" s="9"/>
@@ -41510,7 +41894,9 @@
       <c r="AM67" s="7">
         <v>68</v>
       </c>
-      <c r="AN67" s="7"/>
+      <c r="AN67" s="7">
+        <v>69</v>
+      </c>
       <c r="AO67" s="7"/>
       <c r="AP67" s="7"/>
       <c r="AQ67" s="7"/>
@@ -41804,7 +42190,9 @@
       <c r="AM68" s="15">
         <v>17918</v>
       </c>
-      <c r="AN68" s="15"/>
+      <c r="AN68" s="15">
+        <v>18435</v>
+      </c>
       <c r="AO68" s="15"/>
       <c r="AP68" s="15"/>
       <c r="AQ68" s="15"/>
@@ -42552,6 +42940,9 @@
       <c r="AM72">
         <v>195</v>
       </c>
+      <c r="AN72">
+        <v>201</v>
+      </c>
     </row>
     <row r="73" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="8" t="s">
@@ -42572,6 +42963,9 @@
       <c r="AM73">
         <v>17</v>
       </c>
+      <c r="AN73">
+        <v>18</v>
+      </c>
     </row>
     <row r="74" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="6" t="s">
@@ -42592,6 +42986,9 @@
       <c r="AM74">
         <v>0</v>
       </c>
+      <c r="AN74">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="8" t="s">
@@ -42612,6 +43009,9 @@
       <c r="AM75">
         <v>5</v>
       </c>
+      <c r="AN75">
+        <v>6</v>
+      </c>
     </row>
     <row r="76" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="6" t="s">
@@ -42632,6 +43032,9 @@
       <c r="AM76">
         <v>147</v>
       </c>
+      <c r="AN76">
+        <v>154</v>
+      </c>
     </row>
     <row r="77" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="8" t="s">
@@ -42652,6 +43055,9 @@
       <c r="AM77">
         <v>17</v>
       </c>
+      <c r="AN77">
+        <v>19</v>
+      </c>
     </row>
     <row r="78" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="6" t="s">
@@ -42672,6 +43078,9 @@
       <c r="AM78">
         <v>19</v>
       </c>
+      <c r="AN78">
+        <v>19</v>
+      </c>
     </row>
     <row r="79" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="8" t="s">
@@ -42692,6 +43101,9 @@
       <c r="AM79">
         <v>27</v>
       </c>
+      <c r="AN79">
+        <v>27</v>
+      </c>
     </row>
     <row r="80" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="6" t="s">
@@ -42712,8 +43124,11 @@
       <c r="AM80">
         <v>0</v>
       </c>
+      <c r="AN80">
+        <v>0</v>
+      </c>
     </row>
-    <row r="81" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="8" t="s">
         <v>46</v>
       </c>
@@ -42732,8 +43147,11 @@
       <c r="AM81">
         <v>8</v>
       </c>
+      <c r="AN81">
+        <v>8</v>
+      </c>
     </row>
-    <row r="82" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="6" t="s">
         <v>47</v>
       </c>
@@ -42752,8 +43170,11 @@
       <c r="AM82">
         <v>41</v>
       </c>
+      <c r="AN82">
+        <v>42</v>
+      </c>
     </row>
-    <row r="83" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="8" t="s">
         <v>48</v>
       </c>
@@ -42772,8 +43193,11 @@
       <c r="AM83">
         <v>112</v>
       </c>
+      <c r="AN83">
+        <v>114</v>
+      </c>
     </row>
-    <row r="84" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="6" t="s">
         <v>49</v>
       </c>
@@ -42792,8 +43216,11 @@
       <c r="AM84">
         <v>17</v>
       </c>
+      <c r="AN84">
+        <v>17</v>
+      </c>
     </row>
-    <row r="85" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="8" t="s">
         <v>50</v>
       </c>
@@ -42812,8 +43239,11 @@
       <c r="AM85">
         <v>166</v>
       </c>
+      <c r="AN85">
+        <v>178</v>
+      </c>
     </row>
-    <row r="86" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="6" t="s">
         <v>51</v>
       </c>
@@ -42832,8 +43262,11 @@
       <c r="AM86" s="24" t="s">
         <v>297</v>
       </c>
+      <c r="AN86" s="24" t="s">
+        <v>297</v>
+      </c>
     </row>
-    <row r="87" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="8" t="s">
         <v>52</v>
       </c>
@@ -42852,8 +43285,11 @@
       <c r="AM87">
         <v>102</v>
       </c>
+      <c r="AN87">
+        <v>107</v>
+      </c>
     </row>
-    <row r="88" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="6" t="s">
         <v>53</v>
       </c>
@@ -42872,8 +43308,11 @@
       <c r="AM88" s="24" t="s">
         <v>297</v>
       </c>
+      <c r="AN88" s="24" t="s">
+        <v>297</v>
+      </c>
     </row>
-    <row r="89" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="8" t="s">
         <v>54</v>
       </c>
@@ -42892,8 +43331,11 @@
       <c r="AM89">
         <v>55</v>
       </c>
+      <c r="AN89">
+        <v>56</v>
+      </c>
     </row>
-    <row r="90" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="6" t="s">
         <v>55</v>
       </c>
@@ -42912,8 +43354,11 @@
       <c r="AM90">
         <v>8</v>
       </c>
+      <c r="AN90">
+        <v>8</v>
+      </c>
     </row>
-    <row r="91" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="8" t="s">
         <v>56</v>
       </c>
@@ -42932,8 +43377,11 @@
       <c r="AM91">
         <v>21</v>
       </c>
+      <c r="AN91">
+        <v>21</v>
+      </c>
     </row>
-    <row r="92" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="6" t="s">
         <v>57</v>
       </c>
@@ -42952,8 +43400,11 @@
       <c r="AM92">
         <v>56</v>
       </c>
+      <c r="AN92">
+        <v>57</v>
+      </c>
     </row>
-    <row r="93" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="8" t="s">
         <v>58</v>
       </c>
@@ -42972,8 +43423,11 @@
       <c r="AM93">
         <v>16</v>
       </c>
+      <c r="AN93">
+        <v>19</v>
+      </c>
     </row>
-    <row r="94" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="6" t="s">
         <v>59</v>
       </c>
@@ -42992,8 +43446,11 @@
       <c r="AM94">
         <v>64</v>
       </c>
+      <c r="AN94">
+        <v>66</v>
+      </c>
     </row>
-    <row r="95" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="8" t="s">
         <v>60</v>
       </c>
@@ -43012,8 +43469,11 @@
       <c r="AM95">
         <v>96</v>
       </c>
+      <c r="AN95">
+        <v>100</v>
+      </c>
     </row>
-    <row r="96" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="6" t="s">
         <v>61</v>
       </c>
@@ -43030,6 +43490,9 @@
         <v>297</v>
       </c>
       <c r="AM96" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="AN96" s="24" t="s">
         <v>297</v>
       </c>
     </row>
@@ -43052,6 +43515,9 @@
       <c r="AM97">
         <v>60</v>
       </c>
+      <c r="AN97">
+        <v>65</v>
+      </c>
     </row>
     <row r="98" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="6" t="s">
@@ -43072,6 +43538,9 @@
       <c r="AM98">
         <v>32</v>
       </c>
+      <c r="AN98">
+        <v>32</v>
+      </c>
     </row>
     <row r="99" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="8" t="s">
@@ -43092,6 +43561,9 @@
       <c r="AM99">
         <v>0</v>
       </c>
+      <c r="AN99">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="6" t="s">
@@ -43112,6 +43584,9 @@
       <c r="AM100">
         <v>129</v>
       </c>
+      <c r="AN100">
+        <v>132</v>
+      </c>
     </row>
     <row r="101" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="8" t="s">
@@ -43132,6 +43607,9 @@
       <c r="AM101">
         <v>93</v>
       </c>
+      <c r="AN101">
+        <v>96</v>
+      </c>
     </row>
     <row r="102" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="6" t="s">
@@ -43152,6 +43630,9 @@
       <c r="AM102">
         <v>31</v>
       </c>
+      <c r="AN102">
+        <v>31</v>
+      </c>
     </row>
     <row r="103" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="8" t="s">
@@ -43172,6 +43653,9 @@
       <c r="AM103">
         <v>74</v>
       </c>
+      <c r="AN103">
+        <v>75</v>
+      </c>
     </row>
     <row r="104" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="6" t="s">
@@ -43192,6 +43676,9 @@
       <c r="AM104">
         <v>14</v>
       </c>
+      <c r="AN104">
+        <v>15</v>
+      </c>
     </row>
     <row r="105" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="8" t="s">
@@ -43212,6 +43699,9 @@
       <c r="AM105">
         <v>39</v>
       </c>
+      <c r="AN105">
+        <v>39</v>
+      </c>
     </row>
     <row r="106" spans="1:216" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="10" t="s">
@@ -43231,6 +43721,9 @@
       </c>
       <c r="AM106">
         <v>1666</v>
+      </c>
+      <c r="AN106">
+        <v>1727</v>
       </c>
     </row>
     <row r="107" spans="1:216" ht="17" customHeight="1" x14ac:dyDescent="0.35">
@@ -43472,6 +43965,9 @@
       <c r="AM108">
         <v>0</v>
       </c>
+      <c r="AN108">
+        <v>0</v>
+      </c>
     </row>
     <row r="109" spans="1:216" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
@@ -43492,6 +43988,9 @@
       <c r="AM109">
         <v>0</v>
       </c>
+      <c r="AN109">
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="1:216" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
@@ -43512,6 +44011,9 @@
       <c r="AM110">
         <v>0</v>
       </c>
+      <c r="AN110">
+        <v>0</v>
+      </c>
     </row>
     <row r="111" spans="1:216" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
@@ -43532,6 +44034,9 @@
       <c r="AM111">
         <v>0</v>
       </c>
+      <c r="AN111">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:216" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
@@ -43552,8 +44057,11 @@
       <c r="AM112" s="24">
         <v>3</v>
       </c>
+      <c r="AN112" s="24">
+        <v>3</v>
+      </c>
     </row>
-    <row r="113" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>91</v>
       </c>
@@ -43572,8 +44080,11 @@
       <c r="AM113">
         <v>12</v>
       </c>
+      <c r="AN113">
+        <v>12</v>
+      </c>
     </row>
-    <row r="114" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>92</v>
       </c>
@@ -43592,8 +44103,11 @@
       <c r="AM114">
         <v>29</v>
       </c>
+      <c r="AN114">
+        <v>31</v>
+      </c>
     </row>
-    <row r="115" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>93</v>
       </c>
@@ -43612,8 +44126,11 @@
       <c r="AM115">
         <v>119</v>
       </c>
+      <c r="AN115">
+        <v>123</v>
+      </c>
     </row>
-    <row r="116" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>94</v>
       </c>
@@ -43632,8 +44149,11 @@
       <c r="AM116">
         <v>274</v>
       </c>
+      <c r="AN116">
+        <v>284</v>
+      </c>
     </row>
-    <row r="117" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>95</v>
       </c>
@@ -43652,8 +44172,11 @@
       <c r="AM117">
         <v>1228</v>
       </c>
+      <c r="AN117">
+        <v>1273</v>
+      </c>
     </row>
-    <row r="118" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>96</v>
       </c>
@@ -43672,8 +44195,11 @@
       <c r="AM118" s="24">
         <v>1</v>
       </c>
+      <c r="AN118" s="24">
+        <v>1</v>
+      </c>
     </row>
-    <row r="119" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>97</v>
       </c>
@@ -43690,7 +44216,10 @@
         <v>1562</v>
       </c>
       <c r="AM119" t="s">
-        <v>305</v>
+        <v>303</v>
+      </c>
+      <c r="AN119">
+        <v>1727</v>
       </c>
     </row>
   </sheetData>
@@ -43705,237 +44234,285 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E12"/>
+      <selection activeCell="E4" sqref="E4:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1">
-        <v>167</v>
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>312</v>
       </c>
       <c r="C1" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="D1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
+        <v>314</v>
+      </c>
+      <c r="E1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F1" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2">
-        <v>140</v>
-      </c>
-      <c r="C2" t="s">
-        <v>291</v>
-      </c>
       <c r="D2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+        <v>311</v>
+      </c>
+      <c r="F2" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3">
-        <v>512</v>
-      </c>
-      <c r="C3" t="s">
-        <v>301</v>
-      </c>
       <c r="D3" t="s">
-        <v>310</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>315</v>
+      </c>
+      <c r="F3" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B4">
-        <v>1893</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="D4" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B5">
-        <v>2169</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
       <c r="D5" t="s">
-        <v>313</v>
-      </c>
-      <c r="E5" t="s">
-        <v>297</v>
-      </c>
-      <c r="F5" t="s">
-        <v>290</v>
+        <v>320</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B6">
-        <v>2485</v>
+        <v>528</v>
       </c>
       <c r="C6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D6" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>315</v>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B7">
-        <v>2272</v>
+        <v>1943</v>
       </c>
       <c r="C7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D7" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="E7">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>317</v>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B8">
-        <v>1572</v>
+        <v>2235</v>
       </c>
       <c r="C8" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="D8" t="s">
-        <v>319</v>
-      </c>
-      <c r="E8">
-        <v>119</v>
+        <v>323</v>
+      </c>
+      <c r="E8" t="s">
+        <v>297</v>
       </c>
       <c r="F8" t="s">
-        <v>320</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B9" s="2">
-        <v>1711</v>
+        <v>2545</v>
       </c>
       <c r="C9" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D9" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E9">
-        <v>274</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B10">
-        <v>4929</v>
+        <v>2342</v>
       </c>
       <c r="C10" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D10" t="s">
-        <v>324</v>
-      </c>
-      <c r="E10" t="s">
-        <v>325</v>
+        <v>326</v>
+      </c>
+      <c r="E10">
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B11">
-        <v>68</v>
+        <v>1622</v>
       </c>
       <c r="C11" t="s">
-        <v>229</v>
+        <v>307</v>
       </c>
       <c r="D11" t="s">
-        <v>229</v>
-      </c>
-      <c r="E11" t="s">
-        <v>297</v>
+        <v>328</v>
+      </c>
+      <c r="E11">
+        <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>229</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12">
+        <v>1764</v>
+      </c>
+      <c r="C12" t="s">
+        <v>295</v>
+      </c>
+      <c r="D12" t="s">
+        <v>330</v>
+      </c>
+      <c r="E12">
+        <v>284</v>
+      </c>
+      <c r="F12" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13">
+        <v>5068</v>
+      </c>
+      <c r="C13" t="s">
+        <v>308</v>
+      </c>
+      <c r="D13" t="s">
+        <v>332</v>
+      </c>
+      <c r="E13">
+        <v>1273</v>
+      </c>
+      <c r="F13" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>229</v>
+      </c>
+      <c r="D14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E14" t="s">
+        <v>297</v>
+      </c>
+      <c r="F14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>97</v>
       </c>
-      <c r="B12">
-        <v>17918</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B15">
+        <v>18435</v>
+      </c>
+      <c r="C15" t="s">
         <v>229</v>
       </c>
-      <c r="D12" t="s">
-        <v>304</v>
-      </c>
-      <c r="E12" t="s">
-        <v>305</v>
-      </c>
-      <c r="F12" t="s">
-        <v>327</v>
+      <c r="D15" t="s">
+        <v>309</v>
+      </c>
+      <c r="E15">
+        <v>1727</v>
+      </c>
+      <c r="F15" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="19" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fix active cases data point
</commit_message>
<xml_diff>
--- a/app/data/covid19_MTL.xlsx
+++ b/app/data/covid19_MTL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\code\github\covid19mtl\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECECC9D-D955-43D7-B05E-D25A7684E1AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAED0A86-99E6-4DCA-9889-324EAFBF25A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="390" windowWidth="38620" windowHeight="20740" tabRatio="585" activeTab="2" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
+    <workbookView xWindow="16080" yWindow="5130" windowWidth="21780" windowHeight="12330" tabRatio="585" activeTab="3" xr2:uid="{7101190B-3975-43F4-9365-3E35FA155D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -14867,9 +14867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9609F4-1A5A-459D-8297-63DB4B7007A3}">
   <dimension ref="A1:AS69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC70" sqref="AC70"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26013,9 +26013,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B06CD11-991A-4E1F-B148-C34F5A6BF33A}">
   <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29038,7 +29038,7 @@
         <v>720</v>
       </c>
       <c r="D80">
-        <v>45495</v>
+        <v>28368</v>
       </c>
       <c r="E80">
         <v>3800</v>

</xml_diff>